<commit_message>
Set data validation in excel
</commit_message>
<xml_diff>
--- a/TransporteSerieNacionalFX/src/files/Data.xlsx
+++ b/TransporteSerieNacionalFX/src/files/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gayos\Documents\GitHub\SNB\TransporteSerieNacionalFX\src\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDFCB758-4823-4CD0-A150-8C6F5C8645CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54FCD596-1A84-41A7-9661-4754CFECAE1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -500,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q17"/>
+  <dimension ref="A1:Z17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -511,7 +511,7 @@
     <col min="1" max="1" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -560,8 +560,17 @@
       <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -614,7 +623,7 @@
         <v>1088</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -667,7 +676,7 @@
         <v>951</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -720,7 +729,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -773,7 +782,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -826,7 +835,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -879,7 +888,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -932,7 +941,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -985,7 +994,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -1038,7 +1047,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -1091,7 +1100,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1144,7 +1153,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -1197,7 +1206,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -1250,7 +1259,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1303,7 +1312,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -1410,7 +1419,17 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="s1EjxOWRyVOLOy6c3eCuaslc5mI7Q1lXsr2AnAfuZdwKZcoUIcndwebHzXMVIV7MrkDrntcp8YBqUX//BpiDSg==" saltValue="RMsDpv/x0LToHezcmZoefg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <dataValidations count="3">
+    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Datos erróneos" error="Debe introducir el acrónimo de los_x000a_equipo" promptTitle="Acrónimos de los equipos" sqref="B1:Z1" xr:uid="{2BB70D2A-5F1D-46E4-A333-09933192D084}">
+      <formula1>ISTEXT(B1:Z1)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Datos erróneos" error="Debe introducir el nombre de los equipos" sqref="A2:A26" xr:uid="{E8426092-A3BA-4860-9114-DDE5D0A25DFB}">
+      <formula1>ISTEXT(A2:A26)</formula1>
+    </dataValidation>
+    <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Datos erróneos" error="Debe introducir la distancia entre las sedes de los equipos" sqref="B2:Z26" xr:uid="{EFCFD96C-4502-4865-9FF4-BC5C1FE6F3CD}">
+      <formula1>ISNUMBER(B2:Z26)</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
It's possible to generate a calendar with a odd number of teams
</commit_message>
<xml_diff>
--- a/TransporteSerieNacionalFX/src/files/Data.xlsx
+++ b/TransporteSerieNacionalFX/src/files/Data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gayos\Documents\GitHub\SNB\TransporteSerieNacionalFX\src\files\"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>PRI</t>
   </si>
@@ -121,29 +121,13 @@
   </si>
   <si>
     <t>Guantánamo</t>
-  </si>
-  <si>
-    <t>ASD</t>
-  </si>
-  <si>
-    <t>asd</t>
-  </si>
-  <si>
-    <t>ASR</t>
-  </si>
-  <si>
-    <t>CAR</t>
-  </si>
-  <si>
-    <t>Villa ClaraA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,78 +143,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <b val="true"/>
-      <color indexed="9"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="12.0"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <b val="true"/>
-      <color indexed="9"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="12.0"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <b val="true"/>
-      <color indexed="9"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="12.0"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <b val="true"/>
-      <color indexed="9"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="12.0"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <b val="true"/>
-      <color indexed="9"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="12.0"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <b val="true"/>
-      <color indexed="9"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="12.0"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
-      <b val="true"/>
-      <color indexed="9"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="12.0"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -241,16 +155,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF262626"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="63"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="63"/>
       </patternFill>
     </fill>
   </fills>
@@ -277,39 +181,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -624,7 +500,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P16"/>
+  <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
@@ -632,7 +508,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="1" max="1" width="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
@@ -643,43 +519,46 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="P1" s="14" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
@@ -693,43 +572,46 @@
         <v>130</v>
       </c>
       <c r="D2">
+        <v>170</v>
+      </c>
+      <c r="E2">
         <v>180</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>175</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>280</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>430</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>525</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>455</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>600</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>710</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>835</v>
       </c>
-      <c r="M2">
+      <c r="N2">
+        <v>917</v>
+      </c>
+      <c r="O2">
         <v>915</v>
       </c>
-      <c r="N2">
+      <c r="P2">
         <v>1037</v>
       </c>
-      <c r="O2">
+      <c r="Q2">
         <v>1088</v>
-      </c>
-      <c r="P2" s="15" t="n">
-        <v>1.0</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
@@ -743,693 +625,788 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E3">
         <v>50</v>
       </c>
       <c r="F3">
+        <v>50</v>
+      </c>
+      <c r="G3">
         <v>145</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>295</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>390</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>320</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>465</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>575</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>700</v>
       </c>
-      <c r="M3">
+      <c r="N3">
+        <v>782</v>
+      </c>
+      <c r="O3">
         <v>780</v>
       </c>
-      <c r="N3">
+      <c r="P3">
         <v>902</v>
       </c>
-      <c r="O3">
+      <c r="Q3">
         <v>951</v>
-      </c>
-      <c r="P3" s="15" t="n">
-        <v>142.0</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="C4">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="F4">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="G4">
-        <v>231</v>
+        <v>155</v>
       </c>
       <c r="H4">
-        <v>326</v>
+        <v>305</v>
       </c>
       <c r="I4">
-        <v>256</v>
+        <v>400</v>
       </c>
       <c r="J4">
-        <v>401</v>
+        <v>330</v>
       </c>
       <c r="K4">
-        <v>511</v>
+        <v>475</v>
       </c>
       <c r="L4">
-        <v>636</v>
+        <v>585</v>
       </c>
       <c r="M4">
-        <v>716</v>
+        <v>710</v>
       </c>
       <c r="N4">
-        <v>838</v>
+        <v>792</v>
       </c>
       <c r="O4">
-        <v>887</v>
-      </c>
-      <c r="P4" s="15" t="n">
-        <v>5.0</v>
+        <v>790</v>
+      </c>
+      <c r="P4">
+        <v>912</v>
+      </c>
+      <c r="Q4">
+        <v>961</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="C5">
         <v>50</v>
       </c>
       <c r="D5">
+        <v>40</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
         <v>25</v>
       </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>105</v>
-      </c>
       <c r="G5">
-        <v>255</v>
+        <v>81</v>
       </c>
       <c r="H5">
-        <v>350</v>
+        <v>231</v>
       </c>
       <c r="I5">
-        <v>280</v>
+        <v>326</v>
       </c>
       <c r="J5">
-        <v>425</v>
+        <v>256</v>
       </c>
       <c r="K5">
-        <v>535</v>
+        <v>401</v>
       </c>
       <c r="L5">
-        <v>660</v>
+        <v>511</v>
       </c>
       <c r="M5">
-        <v>740</v>
+        <v>636</v>
       </c>
       <c r="N5">
-        <v>862</v>
+        <v>718</v>
       </c>
       <c r="O5">
-        <v>911</v>
-      </c>
-      <c r="P5" s="15" t="n">
-        <v>2451.0</v>
+        <v>716</v>
+      </c>
+      <c r="P5">
+        <v>838</v>
+      </c>
+      <c r="Q5">
+        <v>887</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6">
+        <v>175</v>
+      </c>
+      <c r="C6">
+        <v>50</v>
+      </c>
+      <c r="D6">
+        <v>70</v>
+      </c>
+      <c r="E6">
+        <v>25</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>105</v>
+      </c>
+      <c r="H6">
+        <v>255</v>
+      </c>
+      <c r="I6">
+        <v>350</v>
+      </c>
+      <c r="J6">
         <v>280</v>
       </c>
-      <c r="C6">
-        <v>145</v>
-      </c>
-      <c r="D6">
-        <v>81</v>
-      </c>
-      <c r="E6">
-        <v>105</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>195</v>
-      </c>
-      <c r="H6">
-        <v>295</v>
-      </c>
-      <c r="I6">
-        <v>220</v>
-      </c>
-      <c r="J6">
-        <v>360</v>
-      </c>
       <c r="K6">
-        <v>480</v>
+        <v>425</v>
       </c>
       <c r="L6">
-        <v>605</v>
+        <v>535</v>
       </c>
       <c r="M6">
-        <v>685</v>
+        <v>660</v>
       </c>
       <c r="N6">
-        <v>807</v>
+        <v>742</v>
       </c>
       <c r="O6">
-        <v>856</v>
-      </c>
-      <c r="P6" s="15" t="n">
-        <v>36.0</v>
+        <v>740</v>
+      </c>
+      <c r="P6">
+        <v>862</v>
+      </c>
+      <c r="Q6">
+        <v>911</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7">
-        <v>430</v>
+        <v>280</v>
       </c>
       <c r="C7">
+        <v>145</v>
+      </c>
+      <c r="D7">
+        <v>155</v>
+      </c>
+      <c r="E7">
+        <v>81</v>
+      </c>
+      <c r="F7">
+        <v>105</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>195</v>
+      </c>
+      <c r="I7">
         <v>295</v>
       </c>
-      <c r="D7">
-        <v>231</v>
-      </c>
-      <c r="E7">
-        <v>255</v>
-      </c>
-      <c r="F7">
-        <v>195</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>155</v>
-      </c>
-      <c r="I7">
-        <v>67</v>
-      </c>
       <c r="J7">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="K7">
-        <v>345</v>
+        <v>360</v>
       </c>
       <c r="L7">
-        <v>470</v>
+        <v>480</v>
       </c>
       <c r="M7">
-        <v>550</v>
+        <v>605</v>
       </c>
       <c r="N7">
-        <v>672</v>
+        <v>687</v>
       </c>
       <c r="O7">
-        <v>721</v>
-      </c>
-      <c r="P7" s="15" t="n">
-        <v>346.0</v>
+        <v>685</v>
+      </c>
+      <c r="P7">
+        <v>807</v>
+      </c>
+      <c r="Q7">
+        <v>856</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8">
-        <v>525</v>
+        <v>430</v>
       </c>
       <c r="C8">
-        <v>390</v>
+        <v>295</v>
       </c>
       <c r="D8">
-        <v>326</v>
+        <v>305</v>
       </c>
       <c r="E8">
-        <v>350</v>
+        <v>231</v>
       </c>
       <c r="F8">
-        <v>295</v>
+        <v>255</v>
       </c>
       <c r="G8">
+        <v>195</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
         <v>155</v>
       </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>85</v>
-      </c>
       <c r="J8">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="K8">
-        <v>195</v>
+        <v>225</v>
       </c>
       <c r="L8">
-        <v>320</v>
+        <v>345</v>
       </c>
       <c r="M8">
-        <v>400</v>
+        <v>470</v>
       </c>
       <c r="N8">
-        <v>522</v>
+        <v>552</v>
       </c>
       <c r="O8">
-        <v>571</v>
-      </c>
-      <c r="P8" s="15" t="n">
-        <v>6.0</v>
+        <v>550</v>
+      </c>
+      <c r="P8">
+        <v>672</v>
+      </c>
+      <c r="Q8">
+        <v>721</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9">
-        <v>455</v>
+        <v>525</v>
       </c>
       <c r="C9">
+        <v>390</v>
+      </c>
+      <c r="D9">
+        <v>400</v>
+      </c>
+      <c r="E9">
+        <v>326</v>
+      </c>
+      <c r="F9">
+        <v>350</v>
+      </c>
+      <c r="G9">
+        <v>295</v>
+      </c>
+      <c r="H9">
+        <v>155</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>85</v>
+      </c>
+      <c r="K9">
+        <v>75</v>
+      </c>
+      <c r="L9">
+        <v>195</v>
+      </c>
+      <c r="M9">
         <v>320</v>
       </c>
-      <c r="D9">
-        <v>256</v>
-      </c>
-      <c r="E9">
-        <v>280</v>
-      </c>
-      <c r="F9">
-        <v>220</v>
-      </c>
-      <c r="G9">
-        <v>67</v>
-      </c>
-      <c r="H9">
-        <v>85</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>160</v>
-      </c>
-      <c r="K9">
-        <v>280</v>
-      </c>
-      <c r="L9">
-        <v>405</v>
-      </c>
-      <c r="M9">
-        <v>485</v>
-      </c>
       <c r="N9">
-        <v>607</v>
+        <v>402</v>
       </c>
       <c r="O9">
-        <v>656</v>
-      </c>
-      <c r="P9" s="15" t="n">
-        <v>647.0</v>
+        <v>400</v>
+      </c>
+      <c r="P9">
+        <v>522</v>
+      </c>
+      <c r="Q9">
+        <v>571</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10">
-        <v>600</v>
+        <v>455</v>
       </c>
       <c r="C10">
-        <v>465</v>
+        <v>320</v>
       </c>
       <c r="D10">
-        <v>401</v>
+        <v>330</v>
       </c>
       <c r="E10">
-        <v>425</v>
+        <v>256</v>
       </c>
       <c r="F10">
-        <v>360</v>
+        <v>280</v>
       </c>
       <c r="G10">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="H10">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="I10">
+        <v>85</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
         <v>160</v>
       </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <v>120</v>
-      </c>
       <c r="L10">
-        <v>245</v>
+        <v>280</v>
       </c>
       <c r="M10">
-        <v>325</v>
+        <v>405</v>
       </c>
       <c r="N10">
-        <v>447</v>
+        <v>487</v>
       </c>
       <c r="O10">
-        <v>496</v>
-      </c>
-      <c r="P10" s="15" t="n">
-        <v>4743.0</v>
+        <v>485</v>
+      </c>
+      <c r="P10">
+        <v>607</v>
+      </c>
+      <c r="Q10">
+        <v>656</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11">
-        <v>710</v>
+        <v>600</v>
       </c>
       <c r="C11">
-        <v>575</v>
+        <v>465</v>
       </c>
       <c r="D11">
-        <v>511</v>
+        <v>475</v>
       </c>
       <c r="E11">
-        <v>535</v>
+        <v>401</v>
       </c>
       <c r="F11">
-        <v>480</v>
+        <v>425</v>
       </c>
       <c r="G11">
-        <v>345</v>
+        <v>360</v>
       </c>
       <c r="H11">
-        <v>195</v>
+        <v>225</v>
       </c>
       <c r="I11">
-        <v>280</v>
+        <v>75</v>
       </c>
       <c r="J11">
+        <v>160</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
         <v>120</v>
       </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <v>125</v>
-      </c>
       <c r="M11">
-        <v>205</v>
+        <v>245</v>
       </c>
       <c r="N11">
         <v>327</v>
       </c>
       <c r="O11">
-        <v>376</v>
-      </c>
-      <c r="P11" s="15" t="n">
-        <v>245.0</v>
+        <v>325</v>
+      </c>
+      <c r="P11">
+        <v>447</v>
+      </c>
+      <c r="Q11">
+        <v>496</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12">
-        <v>835</v>
+        <v>710</v>
       </c>
       <c r="C12">
-        <v>700</v>
+        <v>575</v>
       </c>
       <c r="D12">
-        <v>636</v>
+        <v>585</v>
       </c>
       <c r="E12">
-        <v>660</v>
+        <v>511</v>
       </c>
       <c r="F12">
-        <v>605</v>
+        <v>535</v>
       </c>
       <c r="G12">
-        <v>470</v>
+        <v>480</v>
       </c>
       <c r="H12">
-        <v>320</v>
+        <v>345</v>
       </c>
       <c r="I12">
-        <v>405</v>
+        <v>195</v>
       </c>
       <c r="J12">
-        <v>245</v>
+        <v>280</v>
       </c>
       <c r="K12">
+        <v>120</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
         <v>125</v>
       </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-      <c r="M12">
-        <v>80</v>
-      </c>
       <c r="N12">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="O12">
-        <v>251</v>
-      </c>
-      <c r="P12" s="15" t="n">
-        <v>24.0</v>
+        <v>205</v>
+      </c>
+      <c r="P12">
+        <v>327</v>
+      </c>
+      <c r="Q12">
+        <v>376</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B13">
-        <v>915</v>
+        <v>835</v>
       </c>
       <c r="C13">
-        <v>780</v>
+        <v>700</v>
       </c>
       <c r="D13">
-        <v>716</v>
+        <v>710</v>
       </c>
       <c r="E13">
-        <v>740</v>
+        <v>636</v>
       </c>
       <c r="F13">
-        <v>685</v>
+        <v>660</v>
       </c>
       <c r="G13">
-        <v>550</v>
+        <v>605</v>
       </c>
       <c r="H13">
-        <v>400</v>
+        <v>470</v>
       </c>
       <c r="I13">
-        <v>485</v>
+        <v>320</v>
       </c>
       <c r="J13">
-        <v>325</v>
+        <v>405</v>
       </c>
       <c r="K13">
-        <v>205</v>
+        <v>245</v>
       </c>
       <c r="L13">
+        <v>125</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>82</v>
+      </c>
+      <c r="O13">
         <v>80</v>
       </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
-      <c r="N13">
-        <v>135</v>
-      </c>
-      <c r="O13">
-        <v>185</v>
-      </c>
-      <c r="P13" s="15" t="n">
-        <v>25.0</v>
+      <c r="P13">
+        <v>202</v>
+      </c>
+      <c r="Q13">
+        <v>251</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B14">
-        <v>1037</v>
+        <v>917</v>
       </c>
       <c r="C14">
-        <v>902</v>
+        <v>782</v>
       </c>
       <c r="D14">
-        <v>838</v>
+        <v>792</v>
       </c>
       <c r="E14">
-        <v>862</v>
+        <v>718</v>
       </c>
       <c r="F14">
-        <v>807</v>
+        <v>742</v>
       </c>
       <c r="G14">
-        <v>672</v>
+        <v>687</v>
       </c>
       <c r="H14">
-        <v>522</v>
+        <v>552</v>
       </c>
       <c r="I14">
-        <v>607</v>
+        <v>402</v>
       </c>
       <c r="J14">
-        <v>447</v>
+        <v>487</v>
       </c>
       <c r="K14">
         <v>327</v>
       </c>
       <c r="L14">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="M14">
-        <v>135</v>
+        <v>82</v>
       </c>
       <c r="N14">
         <v>0</v>
       </c>
       <c r="O14">
-        <v>90</v>
-      </c>
-      <c r="P14" s="15" t="n">
-        <v>47.0</v>
+        <v>75</v>
+      </c>
+      <c r="P14">
+        <v>120</v>
+      </c>
+      <c r="Q14">
+        <v>169</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15">
+        <v>915</v>
+      </c>
+      <c r="C15">
+        <v>780</v>
+      </c>
+      <c r="D15">
+        <v>790</v>
+      </c>
+      <c r="E15">
+        <v>716</v>
+      </c>
+      <c r="F15">
+        <v>740</v>
+      </c>
+      <c r="G15">
+        <v>685</v>
+      </c>
+      <c r="H15">
+        <v>550</v>
+      </c>
+      <c r="I15">
+        <v>400</v>
+      </c>
+      <c r="J15">
+        <v>485</v>
+      </c>
+      <c r="K15">
+        <v>325</v>
+      </c>
+      <c r="L15">
+        <v>205</v>
+      </c>
+      <c r="M15">
+        <v>80</v>
+      </c>
+      <c r="N15">
+        <v>75</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>135</v>
+      </c>
+      <c r="Q15">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16">
+        <v>1037</v>
+      </c>
+      <c r="C16">
+        <v>902</v>
+      </c>
+      <c r="D16">
+        <v>912</v>
+      </c>
+      <c r="E16">
+        <v>838</v>
+      </c>
+      <c r="F16">
+        <v>862</v>
+      </c>
+      <c r="G16">
+        <v>807</v>
+      </c>
+      <c r="H16">
+        <v>672</v>
+      </c>
+      <c r="I16">
+        <v>522</v>
+      </c>
+      <c r="J16">
+        <v>607</v>
+      </c>
+      <c r="K16">
+        <v>447</v>
+      </c>
+      <c r="L16">
+        <v>327</v>
+      </c>
+      <c r="M16">
+        <v>202</v>
+      </c>
+      <c r="N16">
+        <v>120</v>
+      </c>
+      <c r="O16">
+        <v>135</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>31</v>
       </c>
-      <c r="B15">
+      <c r="B17">
         <v>1088</v>
       </c>
-      <c r="C15">
+      <c r="C17">
         <v>951</v>
       </c>
-      <c r="D15">
+      <c r="D17">
+        <v>961</v>
+      </c>
+      <c r="E17">
         <v>887</v>
       </c>
-      <c r="E15">
+      <c r="F17">
         <v>911</v>
       </c>
-      <c r="F15">
+      <c r="G17">
         <v>856</v>
       </c>
-      <c r="G15">
+      <c r="H17">
         <v>721</v>
       </c>
-      <c r="H15">
+      <c r="I17">
         <v>571</v>
       </c>
-      <c r="I15">
+      <c r="J17">
         <v>656</v>
       </c>
-      <c r="J15">
+      <c r="K17">
         <v>496</v>
       </c>
-      <c r="K15">
+      <c r="L17">
         <v>376</v>
       </c>
-      <c r="L15">
+      <c r="M17">
         <v>251</v>
       </c>
-      <c r="M15">
+      <c r="N17">
+        <v>169</v>
+      </c>
+      <c r="O17">
         <v>185</v>
       </c>
-      <c r="N15">
+      <c r="P17">
         <v>90</v>
       </c>
-      <c r="O15">
-        <v>0</v>
-      </c>
-      <c r="P15" s="15" t="n">
-        <v>47345.0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" s="15" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="C16" s="15" t="n">
-        <v>142.0</v>
-      </c>
-      <c r="D16" s="15" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="E16" s="15" t="n">
-        <v>2451.0</v>
-      </c>
-      <c r="F16" s="15" t="n">
-        <v>36.0</v>
-      </c>
-      <c r="G16" s="15" t="n">
-        <v>346.0</v>
-      </c>
-      <c r="H16" s="15" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="I16" s="15" t="n">
-        <v>647.0</v>
-      </c>
-      <c r="J16" s="15" t="n">
-        <v>4743.0</v>
-      </c>
-      <c r="K16" s="15" t="n">
-        <v>245.0</v>
-      </c>
-      <c r="L16" s="15" t="n">
-        <v>24.0</v>
-      </c>
-      <c r="M16" s="15" t="n">
-        <v>25.0</v>
-      </c>
-      <c r="N16" s="15" t="n">
-        <v>47.0</v>
-      </c>
-      <c r="O16" s="15" t="n">
-        <v>47345.0</v>
-      </c>
-      <c r="P16" s="15" t="n">
-        <v>0.0</v>
+      <c r="Q17">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>